<commit_message>
11 tests have been written covering 8 cases in the EXCEL spreadsheet.
</commit_message>
<xml_diff>
--- a/doc/TEMPER2 Test coverage.xlsx
+++ b/doc/TEMPER2 Test coverage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymike\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymike\source\repos\Tantrum\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A72184B6-2789-4AB9-B944-A6C6DE84EA60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A4721F-AC40-46F3-89B0-B894341CAC36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{8C0DDD96-B77D-4ED8-9887-F239AB2276E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
   <si>
     <t>Tested in C99</t>
   </si>
@@ -57,12 +57,6 @@
     <t>TEMPER 2 - Coverage</t>
   </si>
   <si>
-    <t>If a test logged any errors, total tests failed increments</t>
-  </si>
-  <si>
-    <t>If a test aborts, total tests aborted increments</t>
-  </si>
-  <si>
     <t>When Temper has NO errors or aborts, the proposed error code is SUCCESS</t>
   </si>
   <si>
@@ -75,12 +69,6 @@
     <t>System coverage</t>
   </si>
   <si>
-    <t>When a test logs any errors it increments the error count for the test correctly</t>
-  </si>
-  <si>
-    <t>When a test aborts, it increments the abort count for the test correctly</t>
-  </si>
-  <si>
     <t>When a parametric is marked as "Should Run", all invokes run</t>
   </si>
   <si>
@@ -136,6 +124,24 @@
   </si>
   <si>
     <t>Test not written</t>
+  </si>
+  <si>
+    <t>Test written</t>
+  </si>
+  <si>
+    <t>When a test triggers any errors it increments the error count for the test correctly</t>
+  </si>
+  <si>
+    <t>If a test triggered any errors, total tests failed increments</t>
+  </si>
+  <si>
+    <t>If a test triggered an aborts, total tests aborted increments</t>
+  </si>
+  <si>
+    <t>If a test is flagged with Skip, total tests skipped increments</t>
+  </si>
+  <si>
+    <t>If a test is flagged with Deprecated, total tests skipped increments</t>
   </si>
 </sst>
 </file>
@@ -183,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -318,11 +324,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -332,20 +347,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -358,6 +363,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FAF15D-6198-4217-81A1-B6966621032C}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,358 +704,370 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>33</v>
+      <c r="C3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>33</v>
+      <c r="C4" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="1" t="s">
+      <c r="C11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="1" t="s">
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="1" t="s">
+      <c r="C18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="3" t="s">
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="3" t="s">
+      <c r="C22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="3" t="s">
+      <c r="C23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="3" t="s">
+      <c r="C24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="3" t="s">
+      <c r="C27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="3" t="s">
+      <c r="C28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="3" t="s">
+      <c r="C29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>33</v>
+      <c r="C30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="A16:A29"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A17:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test coverage for the exit code.
</commit_message>
<xml_diff>
--- a/doc/TEMPER2 Test coverage.xlsx
+++ b/doc/TEMPER2 Test coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymike\source\repos\Tantrum\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A4721F-AC40-46F3-89B0-B894341CAC36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA2F624-EA4F-4FA8-8470-E18BB19DBC87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{8C0DDD96-B77D-4ED8-9887-F239AB2276E4}"/>
+    <workbookView xWindow="44430" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{8C0DDD96-B77D-4ED8-9887-F239AB2276E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,6 +351,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -372,10 +376,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +693,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,15 +704,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -726,175 +726,175 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="21" t="s">
+      <c r="C10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="21" t="s">
+      <c r="C14" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="21" t="s">
+      <c r="C15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -908,7 +908,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
@@ -920,7 +920,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
@@ -932,7 +932,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
@@ -944,7 +944,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
@@ -956,7 +956,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
@@ -968,7 +968,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
@@ -980,7 +980,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
@@ -992,7 +992,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="3" t="s">
         <v>27</v>
       </c>
@@ -1004,7 +1004,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
@@ -1028,7 +1028,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="3" t="s">
         <v>24</v>
       </c>
@@ -1040,7 +1040,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1052,7 +1052,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
CHECK_TRUE and CHECK_FALSE given test coverage
</commit_message>
<xml_diff>
--- a/doc/TEMPER2 Test coverage.xlsx
+++ b/doc/TEMPER2 Test coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymike\source\repos\Tantrum\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA2F624-EA4F-4FA8-8470-E18BB19DBC87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF21F04-950E-4E9B-B8B1-09B5FF3D4E1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44430" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{8C0DDD96-B77D-4ED8-9887-F239AB2276E4}"/>
+    <workbookView xWindow="36000" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{8C0DDD96-B77D-4ED8-9887-F239AB2276E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -337,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -376,6 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +694,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="C30" sqref="C23:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,8 +901,8 @@
       <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>29</v>
+      <c r="C17" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>29</v>
@@ -912,8 +913,8 @@
       <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>29</v>
+      <c r="C18" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>29</v>
@@ -924,8 +925,8 @@
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>29</v>
+      <c r="C19" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>29</v>
@@ -936,8 +937,8 @@
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>29</v>
+      <c r="C20" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>29</v>
@@ -960,7 +961,7 @@
       <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="5" t="s">

</xml_diff>

<commit_message>
Updated the test matrix
</commit_message>
<xml_diff>
--- a/doc/TEMPER2 Test coverage.xlsx
+++ b/doc/TEMPER2 Test coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymike\source\repos\Tantrum\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF21F04-950E-4E9B-B8B1-09B5FF3D4E1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001E26D6-5786-486A-B3E6-C74AAF618756}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{8C0DDD96-B77D-4ED8-9887-F239AB2276E4}"/>
+    <workbookView xWindow="7200" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{8C0DDD96-B77D-4ED8-9887-F239AB2276E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
   <si>
     <t>Tested in C99</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>If a test is flagged with Deprecated, total tests skipped increments</t>
+  </si>
+  <si>
+    <t>Parametric tests can accept structs and classes as params</t>
   </si>
 </sst>
 </file>
@@ -344,7 +347,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -355,6 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FAF15D-6198-4217-81A1-B6966621032C}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C23:C30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,13 +719,13 @@
       <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -731,10 +734,10 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>29</v>
       </c>
     </row>
@@ -743,10 +746,10 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -755,10 +758,10 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -770,7 +773,7 @@
       <c r="C6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -782,7 +785,7 @@
       <c r="C7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -794,138 +797,138 @@
       <c r="C8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="C17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -935,9 +938,9 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -947,10 +950,10 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>29</v>
@@ -959,9 +962,9 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -971,10 +974,10 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>29</v>
@@ -983,10 +986,10 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>29</v>
@@ -995,10 +998,10 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>29</v>
@@ -1007,10 +1010,10 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
       <c r="B26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>29</v>
@@ -1019,10 +1022,10 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>29</v>
@@ -1031,7 +1034,7 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>29</v>
@@ -1042,33 +1045,45 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="7" t="s">
+      <c r="C31" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:A16"/>
-    <mergeCell ref="A17:A30"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="A18:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>